<commit_message>
permit unauthorized access to h2 for dev purposes - h2 has own auth updated example .xlsx file and modified import to account for changed column positions.
</commit_message>
<xml_diff>
--- a/src/main/resources/MedicationLogUpload.xlsx
+++ b/src/main/resources/MedicationLogUpload.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\catha\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ED58BA1-8A85-4777-86DB-F68D33158993}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9836F062-6D75-4F71-8B06-A02707C55E68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3010" yWindow="-110" windowWidth="35500" windowHeight="21820" xr2:uid="{9F186BFD-4414-4B76-A6F8-859374025043}"/>
   </bookViews>
@@ -25,13 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
-  <si>
-    <t>First</t>
-  </si>
-  <si>
-    <t>Second</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
   <si>
     <t>Date</t>
   </si>
@@ -85,6 +79,18 @@
   </si>
   <si>
     <t>palpitations, anxious, feels like rolling MDMA, excess sweating during workout</t>
+  </si>
+  <si>
+    <t>palpitations</t>
+  </si>
+  <si>
+    <t>Dose(mg)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Dose Time</t>
+  </si>
+  <si>
+    <t>Dose Time</t>
   </si>
 </sst>
 </file>
@@ -444,453 +450,570 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EB2C611-5CB2-4DA3-8535-A036389AD9E4}">
-  <dimension ref="A1:K32"/>
+  <dimension ref="A1:L32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="24.81640625" customWidth="1"/>
-    <col min="2" max="2" width="11.08984375" customWidth="1"/>
-    <col min="3" max="3" width="37.6328125" customWidth="1"/>
-    <col min="4" max="4" width="9.26953125" customWidth="1"/>
-    <col min="5" max="5" width="65.453125" customWidth="1"/>
-    <col min="7" max="7" width="43.26953125" customWidth="1"/>
-    <col min="9" max="9" width="12.6328125" customWidth="1"/>
-    <col min="10" max="10" width="11.6328125" customWidth="1"/>
-    <col min="11" max="11" width="14.7265625" customWidth="1"/>
+    <col min="2" max="2" width="37.6328125" customWidth="1"/>
+    <col min="3" max="3" width="11.08984375" customWidth="1"/>
+    <col min="4" max="4" width="10.90625" customWidth="1"/>
+    <col min="5" max="5" width="71.6328125" customWidth="1"/>
+    <col min="6" max="6" width="14.08984375" customWidth="1"/>
+    <col min="7" max="7" width="11.7265625" customWidth="1"/>
+    <col min="8" max="8" width="43.26953125" customWidth="1"/>
+    <col min="10" max="10" width="12.6328125" customWidth="1"/>
+    <col min="11" max="11" width="11.6328125" customWidth="1"/>
+    <col min="12" max="12" width="14.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" t="s">
         <v>14</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>15</v>
       </c>
-      <c r="J1" t="s">
-        <v>16</v>
-      </c>
-      <c r="K1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>45582</v>
       </c>
-      <c r="H2" s="2">
+      <c r="F2">
+        <v>10</v>
+      </c>
+      <c r="I2" s="2">
         <v>0.76875000000000004</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>116</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>71</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>45583</v>
       </c>
-      <c r="B3">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>10</v>
       </c>
       <c r="D3" s="2">
         <v>0.40277777777777779</v>
       </c>
       <c r="E3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="2">
+        <v>7</v>
+      </c>
+      <c r="F3">
+        <v>10</v>
+      </c>
+      <c r="G3" s="2">
         <v>0.58194444444444449</v>
       </c>
-      <c r="G3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" s="2">
+      <c r="H3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" s="2">
         <v>0.39652777777777776</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>125</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>67</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>45584</v>
       </c>
-      <c r="B4">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>10</v>
       </c>
       <c r="D4" s="2">
         <v>0.39583333333333331</v>
       </c>
       <c r="E4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="2">
+        <v>8</v>
+      </c>
+      <c r="F4">
+        <v>10</v>
+      </c>
+      <c r="G4" s="2">
         <v>0.5805555555555556</v>
       </c>
-      <c r="G4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H4" s="2">
+      <c r="H4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4" s="2">
         <v>0.39652777777777776</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>125</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>67</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>45585</v>
       </c>
-      <c r="B5">
+      <c r="C5">
         <v>10</v>
       </c>
       <c r="D5" s="2">
         <v>0.40277777777777779</v>
       </c>
       <c r="E5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="2">
+        <v>9</v>
+      </c>
+      <c r="F5">
+        <v>10</v>
+      </c>
+      <c r="G5" s="2">
         <v>0.6020833333333333</v>
       </c>
-      <c r="G5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H5" s="2">
+      <c r="H5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5" s="2">
         <v>0.39652777777777776</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>125</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>67</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>45586</v>
       </c>
-      <c r="B6">
+      <c r="C6">
         <v>10</v>
       </c>
       <c r="D6" s="2">
         <v>0.43194444444444446</v>
       </c>
       <c r="E6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="2">
+        <v>9</v>
+      </c>
+      <c r="F6">
+        <v>10</v>
+      </c>
+      <c r="G6" s="2">
         <v>0.60416666666666663</v>
       </c>
-      <c r="G6" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6" s="2">
+      <c r="H6" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" s="2">
         <v>0.43125000000000002</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>112</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>62</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>45587</v>
       </c>
-      <c r="B7">
+      <c r="C7">
         <v>10</v>
       </c>
       <c r="D7" s="2">
         <v>0.4236111111111111</v>
       </c>
       <c r="E7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7">
+        <v>10</v>
+      </c>
+      <c r="G7" s="2">
+        <v>0.61597222222222225</v>
+      </c>
+      <c r="H7" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="2">
-        <v>0.61597222222222225</v>
-      </c>
-      <c r="G7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H7" s="2">
+      <c r="I7" s="2">
         <v>0.41249999999999998</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>123</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>78</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>45588</v>
       </c>
-      <c r="B8">
+      <c r="C8">
         <v>10</v>
       </c>
       <c r="D8" s="2">
         <v>0.43194444444444446</v>
       </c>
       <c r="E8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" s="2">
+        <v>11</v>
+      </c>
+      <c r="F8">
+        <v>10</v>
+      </c>
+      <c r="G8" s="2">
         <v>0.61111111111111116</v>
       </c>
-      <c r="G8" t="s">
-        <v>13</v>
-      </c>
-      <c r="H8" s="2">
+      <c r="H8" t="s">
+        <v>11</v>
+      </c>
+      <c r="I8" s="2">
         <v>0.43055555555555558</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>125</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <v>66</v>
       </c>
-      <c r="K8">
+      <c r="L8">
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>45589</v>
       </c>
-      <c r="B9">
+      <c r="C9">
         <v>10</v>
       </c>
       <c r="D9" s="2">
         <v>0.4236111111111111</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9">
+        <v>10</v>
+      </c>
+      <c r="G9" s="2">
         <v>0.59375</v>
       </c>
-      <c r="H9" s="2">
+      <c r="I9" s="2">
         <v>0.41249999999999998</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>119</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>70</v>
       </c>
-      <c r="K9">
+      <c r="L9">
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>45590</v>
       </c>
-      <c r="B10">
+      <c r="C10">
         <v>20</v>
       </c>
       <c r="D10" s="2">
         <v>0.40902777777777777</v>
       </c>
       <c r="E10" t="s">
-        <v>18</v>
-      </c>
-      <c r="F10" s="2">
+        <v>16</v>
+      </c>
+      <c r="F10">
+        <v>20</v>
+      </c>
+      <c r="G10" s="2">
         <v>0.59722222222222221</v>
       </c>
-      <c r="G10" t="s">
-        <v>18</v>
-      </c>
-      <c r="H10" s="2">
+      <c r="I10" s="2">
         <v>0.40763888888888888</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>129</v>
       </c>
-      <c r="J10">
+      <c r="K10">
         <v>68</v>
       </c>
-      <c r="K10">
+      <c r="L10">
         <v>74</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>45591</v>
       </c>
-      <c r="B11">
+      <c r="C11">
         <v>20</v>
       </c>
       <c r="D11" s="2">
         <v>0.41736111111111113</v>
       </c>
       <c r="E11" t="s">
-        <v>18</v>
-      </c>
-      <c r="F11" s="2">
+        <v>16</v>
+      </c>
+      <c r="F11">
+        <v>20</v>
+      </c>
+      <c r="G11" s="2">
         <v>0.64583333333333337</v>
       </c>
-      <c r="G11" t="s">
-        <v>18</v>
-      </c>
-      <c r="H11" s="2">
+      <c r="I11" s="2">
         <v>0.42916666666666664</v>
       </c>
-      <c r="I11">
+      <c r="J11">
         <v>106</v>
       </c>
-      <c r="J11">
+      <c r="K11">
         <v>71</v>
       </c>
-      <c r="K11">
+      <c r="L11">
         <v>68</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="38" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>45592</v>
       </c>
-      <c r="B12">
+      <c r="C12">
         <v>20</v>
       </c>
       <c r="D12" s="2">
         <v>0.40138888888888891</v>
       </c>
       <c r="E12" t="s">
-        <v>19</v>
-      </c>
-      <c r="F12" s="2">
+        <v>17</v>
+      </c>
+      <c r="F12">
+        <v>20</v>
+      </c>
+      <c r="G12" s="2">
         <v>0.58333333333333337</v>
       </c>
-      <c r="H12" s="2">
+      <c r="I12" s="2">
         <v>0.39583333333333331</v>
       </c>
-      <c r="I12">
+      <c r="J12">
         <v>129</v>
       </c>
-      <c r="J12">
+      <c r="K12">
         <v>70</v>
       </c>
-      <c r="K12">
+      <c r="L12">
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A13" s="1"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A14" s="1"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A15" s="1"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A16" s="1"/>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A13" s="1">
+        <v>45593</v>
+      </c>
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13">
+        <v>20</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0.38055555555555554</v>
+      </c>
+      <c r="F13">
+        <v>20</v>
+      </c>
+      <c r="G13" s="2">
+        <v>0.5625</v>
+      </c>
+      <c r="I13" s="2">
+        <v>0.37916666666666665</v>
+      </c>
+      <c r="J13">
+        <v>118</v>
+      </c>
+      <c r="K13">
+        <v>76</v>
+      </c>
+      <c r="L13">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A14" s="1">
+        <v>45594</v>
+      </c>
+      <c r="C14">
+        <v>20</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0.41041666666666665</v>
+      </c>
+      <c r="I14" s="2">
+        <v>0.40902777777777777</v>
+      </c>
+      <c r="J14">
+        <v>133</v>
+      </c>
+      <c r="K14">
+        <v>75</v>
+      </c>
+      <c r="L14">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A15" s="1">
+        <v>45595</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A16" s="1">
+        <v>45596</v>
+      </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A17" s="1"/>
+      <c r="A17" s="1">
+        <v>45597</v>
+      </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A18" s="1"/>
+      <c r="A18" s="1">
+        <v>45598</v>
+      </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A19" s="1"/>
+      <c r="A19" s="1">
+        <v>45599</v>
+      </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A20" s="1"/>
+      <c r="A20" s="1">
+        <v>45600</v>
+      </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A21" s="1"/>
+      <c r="A21" s="1">
+        <v>45601</v>
+      </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A22" s="1"/>
+      <c r="A22" s="1">
+        <v>45602</v>
+      </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A23" s="1"/>
+      <c r="A23" s="1">
+        <v>45603</v>
+      </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A24" s="1"/>
+      <c r="A24" s="1">
+        <v>45604</v>
+      </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A25" s="1"/>
+      <c r="A25" s="1">
+        <v>45605</v>
+      </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A26" s="1"/>
+      <c r="A26" s="1">
+        <v>45606</v>
+      </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A27" s="1"/>
+      <c r="A27" s="1">
+        <v>45607</v>
+      </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A28" s="1"/>
+      <c r="A28" s="1">
+        <v>45608</v>
+      </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A29" s="1"/>
+      <c r="A29" s="1">
+        <v>45609</v>
+      </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A30" s="1"/>
+      <c r="A30" s="1">
+        <v>45610</v>
+      </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A31" s="1"/>
+      <c r="A31" s="1">
+        <v>45611</v>
+      </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A32" s="1"/>
+      <c r="A32" s="1">
+        <v>45612</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
show graph data only for the current user. only upload entries that have relevant data: bloodPressureDiastole, bloodPressureSystole, heartRate
</commit_message>
<xml_diff>
--- a/src/main/resources/MedicationLogUpload.xlsx
+++ b/src/main/resources/MedicationLogUpload.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\catha\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Java\SpringBootProjects\MedTracker\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9836F062-6D75-4F71-8B06-A02707C55E68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{996C472A-F07A-4F42-B741-0E44748A8B7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3010" yWindow="-110" windowWidth="35500" windowHeight="21820" xr2:uid="{9F186BFD-4414-4B76-A6F8-859374025043}"/>
   </bookViews>
@@ -453,7 +453,7 @@
   <dimension ref="A1:L32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -912,6 +912,12 @@
       <c r="D14" s="2">
         <v>0.41041666666666665</v>
       </c>
+      <c r="F14">
+        <v>20</v>
+      </c>
+      <c r="G14" s="2">
+        <v>0.56597222222222221</v>
+      </c>
       <c r="I14" s="2">
         <v>0.40902777777777777</v>
       </c>
@@ -928,6 +934,24 @@
     <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>45595</v>
+      </c>
+      <c r="C15">
+        <v>20</v>
+      </c>
+      <c r="D15" s="2">
+        <v>0.38750000000000001</v>
+      </c>
+      <c r="I15" s="2">
+        <v>0.38472222222222224</v>
+      </c>
+      <c r="J15">
+        <v>107</v>
+      </c>
+      <c r="K15">
+        <v>71</v>
+      </c>
+      <c r="L15">
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.35">

</xml_diff>